<commit_message>
polinom 2nci derece ile sınırlandı
</commit_message>
<xml_diff>
--- a/sonuc_modelleme.xlsx
+++ b/sonuc_modelleme.xlsx
@@ -7,7 +7,7 @@
     <workbookView visibility="visible" minimized="0" showHorizontalScroll="1" showVerticalScroll="1" showSheetTabs="1" tabRatio="600" firstSheet="0" activeTab="0" autoFilterDateGrouping="1"/>
   </bookViews>
   <sheets>
-    <sheet name="Model_Karsilastirma" sheetId="1" state="visible" r:id="rId1"/>
+    <sheet name="Model_Sonuclari" sheetId="1" state="visible" r:id="rId1"/>
     <sheet name="Ham_Veri" sheetId="2" state="visible" r:id="rId2"/>
   </sheets>
   <definedNames/>
@@ -461,7 +461,7 @@
       </c>
       <c r="E1" s="1" t="inlineStr">
         <is>
-          <t>Polinom (3.Der) (%)</t>
+          <t>Polinom (2.Der) (%)</t>
         </is>
       </c>
       <c r="F1" s="1" t="inlineStr">
@@ -478,16 +478,16 @@
         <v>65</v>
       </c>
       <c r="C2" t="n">
-        <v>12.27187182565335</v>
+        <v>11.99841028719179</v>
       </c>
       <c r="D2" t="n">
-        <v>30.38736912121477</v>
+        <v>28.51192875716237</v>
       </c>
       <c r="E2" t="n">
-        <v>26.14332016298203</v>
+        <v>28.29480949943364</v>
       </c>
       <c r="F2" t="n">
-        <v>29.50597969245788</v>
+        <v>28.98751674590322</v>
       </c>
     </row>
     <row r="3">
@@ -501,13 +501,13 @@
         <v>35.41494966270347</v>
       </c>
       <c r="D3" t="n">
-        <v>27.56890719744845</v>
+        <v>26.45229895169499</v>
       </c>
       <c r="E3" t="n">
-        <v>25.87604944752949</v>
+        <v>28.93670644539078</v>
       </c>
       <c r="F3" t="n">
-        <v>25.64495725836142</v>
+        <v>27.61591402048322</v>
       </c>
     </row>
     <row r="4">
@@ -518,16 +518,16 @@
         <v>246</v>
       </c>
       <c r="C4" t="n">
-        <v>25.37825653646057</v>
+        <v>25.37901045048939</v>
       </c>
       <c r="D4" t="n">
-        <v>24.65544093917314</v>
+        <v>24.32324342244781</v>
       </c>
       <c r="E4" t="n">
-        <v>32.01685036921228</v>
+        <v>27.24596210987605</v>
       </c>
       <c r="F4" t="n">
-        <v>23.6877500777047</v>
+        <v>24.89893254032222</v>
       </c>
     </row>
     <row r="5">
@@ -538,16 +538,16 @@
         <v>307</v>
       </c>
       <c r="C5" t="n">
-        <v>22.33270002019254</v>
+        <v>22.33335939214919</v>
       </c>
       <c r="D5" t="n">
-        <v>22.7236861374906</v>
+        <v>22.91158703892523</v>
       </c>
       <c r="E5" t="n">
-        <v>33.64826182071245</v>
+        <v>24.80541519763349</v>
       </c>
       <c r="F5" t="n">
-        <v>22.85124447377626</v>
+        <v>23.05668112579334</v>
       </c>
     </row>
     <row r="6">
@@ -558,16 +558,16 @@
         <v>368</v>
       </c>
       <c r="C6" t="n">
-        <v>19.28714350392452</v>
+        <v>19.28770833380899</v>
       </c>
       <c r="D6" t="n">
-        <v>20.79193133580807</v>
+        <v>21.49993065540264</v>
       </c>
       <c r="E6" t="n">
-        <v>29.07717629400858</v>
+        <v>21.31271005875625</v>
       </c>
       <c r="F6" t="n">
-        <v>22.1617300229743</v>
+        <v>21.36207068986936</v>
       </c>
     </row>
     <row r="7">
@@ -578,16 +578,16 @@
         <v>425</v>
       </c>
       <c r="C7" t="n">
-        <v>16.44129561167406</v>
+        <v>16.44177209896651</v>
       </c>
       <c r="D7" t="n">
-        <v>18.98684898013749</v>
+        <v>20.18084190358646</v>
       </c>
       <c r="E7" t="n">
-        <v>15.982123533806</v>
+        <v>17.09810541375526</v>
       </c>
       <c r="F7" t="n">
-        <v>21.57063874120238</v>
+        <v>19.95433944690444</v>
       </c>
     </row>
   </sheetData>
@@ -644,7 +644,7 @@
         <v>46006</v>
       </c>
       <c r="D2" t="n">
-        <v>39.49999999999998</v>
+        <v>33.57499999999958</v>
       </c>
     </row>
     <row r="3">
@@ -708,7 +708,7 @@
         <v>46246</v>
       </c>
       <c r="D6" t="n">
-        <v>25.52803800447375</v>
+        <v>25.52879656811268</v>
       </c>
     </row>
     <row r="7">
@@ -724,7 +724,7 @@
         <v>46428</v>
       </c>
       <c r="D7" t="n">
-        <v>16.44129561167406</v>
+        <v>16.44177209896651</v>
       </c>
     </row>
   </sheetData>

</xml_diff>